<commit_message>
Update on 20250411 part 8
</commit_message>
<xml_diff>
--- a/直播源汇总文档/各地组播源汇总/江西.xlsx
+++ b/直播源汇总文档/各地组播源汇总/江西.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="59">
   <si>
     <t>江西都市</t>
   </si>
@@ -196,6 +196,18 @@
   </si>
   <si>
     <t>IPB</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>/rtp/239.252.220.241:5140</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>/rtp/239.252.219.115:5140</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>江西教育</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -557,7 +569,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E47"/>
+  <dimension ref="A1:E49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1366,7 +1378,41 @@
         <v>55</v>
       </c>
       <c r="E47" t="s">
-        <v>13</v>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A48" t="s">
+        <v>58</v>
+      </c>
+      <c r="B48" t="s">
+        <v>16</v>
+      </c>
+      <c r="C48" t="s">
+        <v>17</v>
+      </c>
+      <c r="D48" t="s">
+        <v>18</v>
+      </c>
+      <c r="E48" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A49" t="s">
+        <v>58</v>
+      </c>
+      <c r="B49" t="s">
+        <v>16</v>
+      </c>
+      <c r="C49" t="s">
+        <v>17</v>
+      </c>
+      <c r="D49" t="s">
+        <v>55</v>
+      </c>
+      <c r="E49" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>